<commit_message>
Git lfs track a couple folders
</commit_message>
<xml_diff>
--- a/PokemonFinal.xlsx
+++ b/PokemonFinal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="259">
   <si>
     <t>ID</t>
   </si>
@@ -229,9 +229,15 @@
     <t>Ekans</t>
   </si>
   <si>
+    <t>Toxic 1</t>
+  </si>
+  <si>
     <t>Arbok</t>
   </si>
   <si>
+    <t>Glare</t>
+  </si>
+  <si>
     <t>Pikachu</t>
   </si>
   <si>
@@ -313,9 +319,6 @@
     <t>Zubat</t>
   </si>
   <si>
-    <t>Toxic 1</t>
-  </si>
-  <si>
     <t>Golbat</t>
   </si>
   <si>
@@ -460,6 +463,9 @@
     <t>Armored 3</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Ponyta</t>
   </si>
   <si>
@@ -655,6 +661,9 @@
     <t>Mr. Mime</t>
   </si>
   <si>
+    <t>Mimic</t>
+  </si>
+  <si>
     <t>Scyther</t>
   </si>
   <si>
@@ -674,9 +683,6 @@
   </si>
   <si>
     <t>Pinsir</t>
-  </si>
-  <si>
-    <t>4</t>
   </si>
   <si>
     <t>Tauros</t>
@@ -929,9 +935,6 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -940,6 +943,9 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -2007,7 +2013,7 @@
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="8">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="10"/>
@@ -2115,11 +2121,11 @@
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="16" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="8">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I24" s="11" t="s">
         <v>54</v>
@@ -2145,7 +2151,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>67</v>
@@ -2154,14 +2160,16 @@
         <v>51</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="19"/>
+      <c r="F25" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="H25" s="8">
         <v>7.0</v>
       </c>
-      <c r="I25" s="20"/>
+      <c r="I25" s="19"/>
       <c r="J25" s="10"/>
       <c r="K25" s="8">
         <v>1.0</v>
@@ -2181,13 +2189,13 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -2199,7 +2207,7 @@
         <v>17</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K26" s="8">
         <v>0.0</v>
@@ -2219,13 +2227,13 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="14" t="s">
@@ -2255,17 +2263,17 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="8">
@@ -2295,20 +2303,20 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H29" s="8">
         <v>8.0</v>
@@ -2332,8 +2340,8 @@
       <c r="A30" s="8">
         <v>29.0</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>79</v>
+      <c r="B30" s="20" t="s">
+        <v>81</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>15</v>
@@ -2371,7 +2379,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>21</v>
@@ -2381,7 +2389,7 @@
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="8">
@@ -2389,7 +2397,7 @@
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K31" s="8">
         <v>1.0</v>
@@ -2409,22 +2417,22 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="H32" s="8">
         <v>9.0</v>
@@ -2448,8 +2456,8 @@
       <c r="A33" s="8">
         <v>32.0</v>
       </c>
-      <c r="B33" s="22" t="s">
-        <v>84</v>
+      <c r="B33" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>15</v>
@@ -2487,7 +2495,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>21</v>
@@ -2497,7 +2505,7 @@
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G34" s="10"/>
       <c r="H34" s="8">
@@ -2505,7 +2513,7 @@
       </c>
       <c r="I34" s="15"/>
       <c r="J34" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K34" s="8">
         <v>1.0</v>
@@ -2525,22 +2533,22 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H35" s="8">
         <v>9.0</v>
@@ -2565,7 +2573,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>21</v>
@@ -2583,7 +2591,7 @@
         <v>58</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K36" s="8">
         <v>0.0</v>
@@ -2605,7 +2613,7 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>67</v>
@@ -2615,13 +2623,13 @@
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H37" s="8">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="I37" s="15"/>
       <c r="J37" s="10"/>
@@ -2643,7 +2651,7 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>15</v>
@@ -2661,7 +2669,7 @@
         <v>54</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K38" s="8">
         <v>0.0</v>
@@ -2681,7 +2689,7 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>67</v>
@@ -2717,7 +2725,7 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>15</v>
@@ -2737,7 +2745,7 @@
         <v>54</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K40" s="8">
         <v>0.0</v>
@@ -2757,7 +2765,7 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>21</v>
@@ -2767,7 +2775,7 @@
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>47</v>
@@ -2795,7 +2803,7 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>15</v>
@@ -2807,7 +2815,7 @@
         <v>46</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="G42" s="10"/>
       <c r="H42" s="8">
@@ -2817,7 +2825,7 @@
         <v>54</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="K42" s="8">
         <v>0.0</v>
@@ -2837,7 +2845,7 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>21</v>
@@ -2855,7 +2863,7 @@
         <v>52</v>
       </c>
       <c r="H43" s="8">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="10"/>
@@ -2877,7 +2885,7 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>15</v>
@@ -2889,7 +2897,7 @@
         <v>51</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="G44" s="10"/>
       <c r="H44" s="8">
@@ -2919,7 +2927,7 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>21</v>
@@ -2939,7 +2947,7 @@
       </c>
       <c r="I45" s="15"/>
       <c r="J45" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K45" s="8">
         <v>1.0</v>
@@ -2959,7 +2967,7 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>25</v>
@@ -2971,7 +2979,7 @@
         <v>51</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="8">
@@ -2997,7 +3005,7 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>15</v>
@@ -3041,7 +3049,7 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>21</v>
@@ -3053,13 +3061,13 @@
         <v>16</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G48" s="10"/>
       <c r="H48" s="8">
         <v>6.0</v>
       </c>
-      <c r="I48" s="20"/>
+      <c r="I48" s="19"/>
       <c r="J48" s="10"/>
       <c r="K48" s="8">
         <v>1.0</v>
@@ -3079,7 +3087,7 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>15</v>
@@ -3091,7 +3099,7 @@
         <v>51</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="G49" s="10"/>
       <c r="H49" s="8">
@@ -3121,7 +3129,7 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>67</v>
@@ -3161,17 +3169,17 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E51" s="10"/>
       <c r="F51" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G51" s="10"/>
       <c r="H51" s="8">
@@ -3201,25 +3209,25 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E52" s="10"/>
       <c r="F52" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>57</v>
       </c>
       <c r="H52" s="18">
-        <v>8.0</v>
-      </c>
-      <c r="I52" s="20"/>
+        <v>7.0</v>
+      </c>
+      <c r="I52" s="19"/>
       <c r="J52" s="10"/>
       <c r="K52" s="8">
         <v>1.0</v>
@@ -3241,7 +3249,7 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>21</v>
@@ -3251,14 +3259,14 @@
       </c>
       <c r="E53" s="10"/>
       <c r="F53" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G53" s="10"/>
       <c r="H53" s="8">
         <v>3.0</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J53" s="8" t="s">
         <v>44</v>
@@ -3281,7 +3289,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>67</v>
@@ -3317,7 +3325,7 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>15</v>
@@ -3355,25 +3363,25 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G56" s="10"/>
       <c r="H56" s="8">
         <v>8.0</v>
       </c>
-      <c r="I56" s="20"/>
+      <c r="I56" s="19"/>
       <c r="J56" s="10"/>
       <c r="K56" s="8">
         <v>1.0</v>
@@ -3393,13 +3401,13 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
@@ -3433,23 +3441,23 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G58" s="10"/>
       <c r="H58" s="8">
         <v>8.0</v>
       </c>
-      <c r="I58" s="20"/>
+      <c r="I58" s="19"/>
       <c r="J58" s="10"/>
       <c r="K58" s="8">
         <v>1.0</v>
@@ -3469,7 +3477,7 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>67</v>
@@ -3487,7 +3495,7 @@
         <v>58</v>
       </c>
       <c r="J59" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K59" s="8">
         <v>0.0</v>
@@ -3507,7 +3515,7 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>25</v>
@@ -3519,7 +3527,7 @@
       <c r="F60" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G60" s="19"/>
+      <c r="G60" s="22"/>
       <c r="H60" s="8">
         <v>11.0</v>
       </c>
@@ -3543,10 +3551,10 @@
         <v>60.0</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>33</v>
@@ -3557,7 +3565,7 @@
       </c>
       <c r="G61" s="10"/>
       <c r="H61" s="8">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I61" s="11" t="s">
         <v>54</v>
@@ -3583,10 +3591,10 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>33</v>
@@ -3599,7 +3607,7 @@
       </c>
       <c r="I62" s="15"/>
       <c r="J62" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K62" s="8">
         <v>1.0</v>
@@ -3619,23 +3627,23 @@
         <v>62.0</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G63" s="10"/>
       <c r="H63" s="8">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="I63" s="15"/>
       <c r="J63" s="10"/>
@@ -3657,13 +3665,13 @@
         <v>63.0</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
@@ -3695,17 +3703,17 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E65" s="10"/>
       <c r="F65" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G65" s="10"/>
       <c r="H65" s="18">
@@ -3733,17 +3741,17 @@
         <v>65.0</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E66" s="10"/>
       <c r="F66" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G66" s="10"/>
       <c r="H66" s="8">
@@ -3769,17 +3777,17 @@
         <v>66.0</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G67" s="10"/>
       <c r="H67" s="8">
@@ -3809,24 +3817,24 @@
         <v>67.0</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E68" s="10"/>
       <c r="F68" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G68" s="10"/>
       <c r="H68" s="8">
         <v>6.0</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J68" s="8" t="s">
         <v>25</v>
@@ -3849,24 +3857,24 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E69" s="10"/>
       <c r="F69" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G69" s="10"/>
       <c r="H69" s="8">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J69" s="10"/>
       <c r="K69" s="8">
@@ -3887,7 +3895,7 @@
         <v>69.0</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>15</v>
@@ -3926,8 +3934,8 @@
       <c r="A71" s="8">
         <v>70.0</v>
       </c>
-      <c r="B71" s="22" t="s">
-        <v>136</v>
+      <c r="B71" s="21" t="s">
+        <v>137</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>21</v>
@@ -3945,7 +3953,7 @@
       </c>
       <c r="I71" s="15"/>
       <c r="J71" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K71" s="8">
         <v>1.0</v>
@@ -3964,8 +3972,8 @@
       <c r="A72" s="8">
         <v>71.0</v>
       </c>
-      <c r="B72" s="22" t="s">
-        <v>137</v>
+      <c r="B72" s="21" t="s">
+        <v>138</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>25</v>
@@ -3975,9 +3983,9 @@
       </c>
       <c r="E72" s="10"/>
       <c r="F72" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="G72" s="19"/>
+        <v>139</v>
+      </c>
+      <c r="G72" s="22"/>
       <c r="H72" s="8">
         <v>9.0</v>
       </c>
@@ -4001,7 +4009,7 @@
         <v>72.0</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>67</v>
@@ -4012,8 +4020,8 @@
       <c r="E73" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F73" s="16" t="s">
-        <v>22</v>
+      <c r="F73" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="G73" s="10"/>
       <c r="H73" s="8">
@@ -4043,7 +4051,7 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>25</v>
@@ -4057,9 +4065,9 @@
       <c r="F74" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G74" s="19"/>
+      <c r="G74" s="22"/>
       <c r="H74" s="18">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="I74" s="15"/>
       <c r="J74" s="10"/>
@@ -4081,13 +4089,13 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E75" s="10"/>
       <c r="F75" s="14" t="s">
@@ -4121,13 +4129,13 @@
         <v>75.0</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E76" s="10"/>
       <c r="F76" s="14" t="s">
@@ -4135,10 +4143,10 @@
       </c>
       <c r="G76" s="10"/>
       <c r="H76" s="8">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J76" s="8" t="s">
         <v>25</v>
@@ -4163,24 +4171,26 @@
         <v>76.0</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E77" s="10"/>
+        <v>143</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="F77" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G77" s="10"/>
       <c r="H77" s="8">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="J77" s="10"/>
       <c r="K77" s="8">
@@ -4201,7 +4211,7 @@
         <v>77.0</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>21</v>
@@ -4211,7 +4221,7 @@
       </c>
       <c r="E78" s="10"/>
       <c r="F78" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G78" s="10"/>
       <c r="H78" s="8">
@@ -4241,7 +4251,7 @@
         <v>78.0</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>25</v>
@@ -4251,7 +4261,7 @@
       </c>
       <c r="E79" s="10"/>
       <c r="F79" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G79" s="14" t="s">
         <v>30</v>
@@ -4279,13 +4289,13 @@
         <v>79.0</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>33</v>
@@ -4319,25 +4329,25 @@
         <v>80.0</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G81" s="10"/>
       <c r="H81" s="8">
         <v>9.0</v>
       </c>
-      <c r="I81" s="20"/>
+      <c r="I81" s="19"/>
       <c r="J81" s="10"/>
       <c r="K81" s="8">
         <v>1.0</v>
@@ -4357,22 +4367,22 @@
         <v>81.0</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E82" s="10"/>
-      <c r="F82" s="19"/>
+      <c r="F82" s="22"/>
       <c r="G82" s="10"/>
       <c r="H82" s="8">
         <v>4.0</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J82" s="8" t="s">
         <v>18</v>
@@ -4397,17 +4407,17 @@
         <v>82.0</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E83" s="10"/>
       <c r="F83" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G83" s="10"/>
       <c r="H83" s="18">
@@ -4433,7 +4443,7 @@
         <v>83.0</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>21</v>
@@ -4443,14 +4453,14 @@
       </c>
       <c r="E84" s="10"/>
       <c r="F84" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G84" s="10"/>
       <c r="H84" s="8">
         <v>5.0</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J84" s="10"/>
       <c r="K84" s="8">
@@ -4471,7 +4481,7 @@
         <v>84.0</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>15</v>
@@ -4483,7 +4493,7 @@
         <v>62</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G85" s="10"/>
       <c r="H85" s="8">
@@ -4513,7 +4523,7 @@
         <v>85.0</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>67</v>
@@ -4525,13 +4535,13 @@
         <v>62</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G86" s="10"/>
       <c r="H86" s="8">
         <v>8.0</v>
       </c>
-      <c r="I86" s="20"/>
+      <c r="I86" s="19"/>
       <c r="J86" s="10"/>
       <c r="K86" s="8">
         <v>1.0</v>
@@ -4551,7 +4561,7 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>21</v>
@@ -4561,7 +4571,7 @@
       </c>
       <c r="E87" s="10"/>
       <c r="F87" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G87" s="10"/>
       <c r="H87" s="8">
@@ -4591,26 +4601,26 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G88" s="10"/>
       <c r="H88" s="8">
         <v>9.0</v>
       </c>
       <c r="I88" s="11" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="8">
@@ -4633,7 +4643,7 @@
         <v>88.0</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>67</v>
@@ -4643,7 +4653,7 @@
       </c>
       <c r="E89" s="10"/>
       <c r="F89" s="14" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="G89" s="10"/>
       <c r="H89" s="8">
@@ -4673,7 +4683,7 @@
         <v>89.0</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>25</v>
@@ -4683,11 +4693,11 @@
       </c>
       <c r="E90" s="10"/>
       <c r="F90" s="14" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G90" s="10"/>
       <c r="H90" s="8">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="I90" s="15"/>
       <c r="J90" s="10"/>
@@ -4709,10 +4719,10 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>33</v>
@@ -4726,10 +4736,10 @@
         <v>3.0</v>
       </c>
       <c r="I91" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J91" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K91" s="8">
         <v>0.0</v>
@@ -4749,23 +4759,23 @@
         <v>91.0</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G92" s="10"/>
       <c r="H92" s="8">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="I92" s="15"/>
       <c r="J92" s="10"/>
@@ -4787,13 +4797,13 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E93" s="10"/>
       <c r="F93" s="10"/>
@@ -4802,7 +4812,7 @@
         <v>4.0</v>
       </c>
       <c r="I93" s="11" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J93" s="8" t="s">
         <v>67</v>
@@ -4825,13 +4835,13 @@
         <v>93.0</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E94" s="10"/>
       <c r="F94" s="10"/>
@@ -4840,7 +4850,7 @@
         <v>7.0</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J94" s="8" t="s">
         <v>25</v>
@@ -4863,24 +4873,24 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E95" s="10"/>
       <c r="F95" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G95" s="10"/>
       <c r="H95" s="8">
         <v>11.0</v>
       </c>
       <c r="I95" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J95" s="10"/>
       <c r="K95" s="8">
@@ -4901,26 +4911,26 @@
         <v>95.0</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F96" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="G96" s="19"/>
+        <v>139</v>
+      </c>
+      <c r="G96" s="22"/>
       <c r="H96" s="8">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="I96" s="11" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="J96" s="10"/>
       <c r="K96" s="8">
@@ -4941,13 +4951,13 @@
         <v>96.0</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E97" s="10"/>
       <c r="F97" s="8" t="s">
@@ -4981,17 +4991,17 @@
         <v>97.0</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E98" s="10"/>
       <c r="F98" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G98" s="8" t="s">
         <v>47</v>
@@ -5019,7 +5029,7 @@
         <v>98.0</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>21</v>
@@ -5059,7 +5069,7 @@
         <v>99.0</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>67</v>
@@ -5069,7 +5079,7 @@
       </c>
       <c r="E100" s="10"/>
       <c r="F100" s="14" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G100" s="10"/>
       <c r="H100" s="8">
@@ -5095,17 +5105,17 @@
         <v>100.0</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E101" s="10"/>
       <c r="F101" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G101" s="10"/>
       <c r="H101" s="8">
@@ -5135,17 +5145,17 @@
         <v>101.0</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E102" s="10"/>
       <c r="F102" s="8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G102" s="10"/>
       <c r="H102" s="8">
@@ -5171,18 +5181,18 @@
         <v>102.0</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F103" s="19"/>
+      <c r="F103" s="22"/>
       <c r="G103" s="10"/>
       <c r="H103" s="8">
         <v>4.0</v>
@@ -5191,7 +5201,7 @@
         <v>58</v>
       </c>
       <c r="J103" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K103" s="8">
         <v>0.0</v>
@@ -5211,23 +5221,23 @@
         <v>103.0</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E104" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G104" s="10"/>
       <c r="H104" s="18">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="I104" s="15"/>
       <c r="J104" s="10"/>
@@ -5249,13 +5259,13 @@
         <v>104.0</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E105" s="10"/>
       <c r="F105" s="8" t="s">
@@ -5289,21 +5299,21 @@
         <v>105.0</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E106" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F106" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G106" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G106" s="22"/>
       <c r="H106" s="8">
         <v>7.0</v>
       </c>
@@ -5327,24 +5337,24 @@
         <v>106.0</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E107" s="10"/>
       <c r="F107" s="14" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G107" s="10"/>
       <c r="H107" s="8">
         <v>7.0</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="J107" s="10"/>
       <c r="K107" s="8">
@@ -5365,24 +5375,24 @@
         <v>107.0</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E108" s="10"/>
       <c r="F108" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G108" s="10"/>
       <c r="H108" s="8">
         <v>7.0</v>
       </c>
       <c r="I108" s="11" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="J108" s="10"/>
       <c r="K108" s="8">
@@ -5403,7 +5413,7 @@
         <v>108.0</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>21</v>
@@ -5413,14 +5423,14 @@
       </c>
       <c r="E109" s="10"/>
       <c r="F109" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G109" s="10"/>
       <c r="H109" s="18">
         <v>6.0</v>
       </c>
       <c r="I109" s="11" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="8">
@@ -5441,7 +5451,7 @@
         <v>109.0</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>21</v>
@@ -5451,7 +5461,7 @@
       </c>
       <c r="E110" s="10"/>
       <c r="F110" s="14" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="G110" s="10"/>
       <c r="H110" s="8">
@@ -5481,7 +5491,7 @@
         <v>110.0</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>67</v>
@@ -5491,7 +5501,7 @@
       </c>
       <c r="E111" s="10"/>
       <c r="F111" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G111" s="10"/>
       <c r="H111" s="8">
@@ -5517,16 +5527,16 @@
         <v>111.0</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F112" s="10"/>
       <c r="G112" s="10"/>
@@ -5537,7 +5547,7 @@
         <v>58</v>
       </c>
       <c r="J112" s="8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K112" s="8">
         <v>0.0</v>
@@ -5557,19 +5567,19 @@
         <v>112.0</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F113" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G113" s="10"/>
       <c r="H113" s="8">
@@ -5595,26 +5605,26 @@
         <v>113.0</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E114" s="10"/>
       <c r="F114" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H114" s="8">
         <v>7.0</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="J114" s="10"/>
       <c r="K114" s="8">
@@ -5635,7 +5645,7 @@
         <v>114.0</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>21</v>
@@ -5649,7 +5659,7 @@
       </c>
       <c r="G115" s="10"/>
       <c r="H115" s="8">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="I115" s="11" t="s">
         <v>58</v>
@@ -5673,7 +5683,7 @@
         <v>115.0</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>25</v>
@@ -5683,14 +5693,14 @@
       </c>
       <c r="E116" s="10"/>
       <c r="F116" s="18" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G116" s="10"/>
       <c r="H116" s="8">
         <v>9.0</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="J116" s="10"/>
       <c r="K116" s="8">
@@ -5711,7 +5721,7 @@
         <v>116.0</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>15</v>
@@ -5751,19 +5761,19 @@
         <v>117.0</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E118" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F118" s="14" t="s">
         <v>162</v>
-      </c>
-      <c r="F118" s="14" t="s">
-        <v>160</v>
       </c>
       <c r="G118" s="10"/>
       <c r="H118" s="8">
@@ -5789,7 +5799,7 @@
         <v>118.0</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>15</v>
@@ -5829,17 +5839,17 @@
         <v>119.0</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E120" s="10"/>
       <c r="F120" s="14" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G120" s="10"/>
       <c r="H120" s="8">
@@ -5865,7 +5875,7 @@
         <v>120.0</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>67</v>
@@ -5874,7 +5884,7 @@
         <v>33</v>
       </c>
       <c r="E121" s="10"/>
-      <c r="F121" s="19"/>
+      <c r="F121" s="22"/>
       <c r="G121" s="10"/>
       <c r="H121" s="8">
         <v>5.0</v>
@@ -5883,7 +5893,7 @@
         <v>58</v>
       </c>
       <c r="J121" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K121" s="8">
         <v>0.0</v>
@@ -5903,7 +5913,7 @@
         <v>121.0</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>25</v>
@@ -5912,7 +5922,7 @@
         <v>33</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F122" s="14" t="s">
         <v>64</v>
@@ -5941,24 +5951,24 @@
         <v>122.0</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E123" s="10"/>
-      <c r="F123" s="14" t="s">
-        <v>35</v>
+      <c r="F123" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="G123" s="10"/>
       <c r="H123" s="18">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="I123" s="11" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J123" s="10"/>
       <c r="K123" s="8">
@@ -5979,7 +5989,7 @@
         <v>123.0</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>25</v>
@@ -5991,14 +6001,14 @@
         <v>46</v>
       </c>
       <c r="F124" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G124" s="10"/>
       <c r="H124" s="8">
         <v>9.0</v>
       </c>
       <c r="I124" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="8">
@@ -6019,26 +6029,26 @@
         <v>124.0</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F125" s="14" t="s">
-        <v>160</v>
+        <v>115</v>
+      </c>
+      <c r="F125" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="G125" s="10"/>
       <c r="H125" s="8">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="I125" s="11" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J125" s="10"/>
       <c r="K125" s="8">
@@ -6059,24 +6069,24 @@
         <v>125.0</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C126" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E126" s="10"/>
       <c r="F126" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G126" s="10"/>
       <c r="H126" s="8">
         <v>9.0</v>
       </c>
       <c r="I126" s="11" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="J126" s="10"/>
       <c r="K126" s="17">
@@ -6097,7 +6107,7 @@
         <v>126.0</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>67</v>
@@ -6114,7 +6124,7 @@
         <v>9.0</v>
       </c>
       <c r="I127" s="11" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="17">
@@ -6135,7 +6145,7 @@
         <v>127.0</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>25</v>
@@ -6145,14 +6155,14 @@
       </c>
       <c r="E128" s="10"/>
       <c r="F128" s="14" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G128" s="10"/>
       <c r="H128" s="8">
         <v>9.0</v>
       </c>
       <c r="I128" s="11" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="J128" s="10"/>
       <c r="K128" s="17">
@@ -6173,7 +6183,7 @@
         <v>128.0</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>25</v>
@@ -6183,14 +6193,14 @@
       </c>
       <c r="E129" s="10"/>
       <c r="F129" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G129" s="10"/>
       <c r="H129" s="8">
         <v>10.0</v>
       </c>
       <c r="I129" s="11" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="J129" s="10"/>
       <c r="K129" s="17">
@@ -6211,7 +6221,7 @@
         <v>129.0</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>21</v>
@@ -6249,19 +6259,19 @@
         <v>130.0</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C131" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F131" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G131" s="10"/>
       <c r="H131" s="8">
@@ -6287,24 +6297,24 @@
         <v>131.0</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E132" s="10"/>
       <c r="F132" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G132" s="10"/>
       <c r="H132" s="8">
         <v>10.0</v>
       </c>
       <c r="I132" s="11" t="s">
-        <v>218</v>
+        <v>135</v>
       </c>
       <c r="J132" s="10"/>
       <c r="K132" s="17">
@@ -6325,7 +6335,7 @@
         <v>132.0</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>67</v>
@@ -6335,7 +6345,7 @@
       </c>
       <c r="E133" s="10"/>
       <c r="F133" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G133" s="10"/>
       <c r="H133" s="8">
@@ -6363,7 +6373,7 @@
         <v>133.0</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C134" s="8" t="s">
         <v>15</v>
@@ -6378,17 +6388,17 @@
         <v>4.0</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J134" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K134" s="17">
         <v>0.0</v>
       </c>
       <c r="L134" s="12"/>
       <c r="M134" s="7" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="N134" s="13" t="str">
         <f t="shared" si="2"/>
@@ -6400,7 +6410,7 @@
         <v>134.0</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C135" s="8" t="s">
         <v>25</v>
@@ -6410,7 +6420,7 @@
       </c>
       <c r="E135" s="10"/>
       <c r="F135" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G135" s="10"/>
       <c r="H135" s="8">
@@ -6436,13 +6446,13 @@
         <v>135.0</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E136" s="10"/>
       <c r="F136" s="14" t="s">
@@ -6472,7 +6482,7 @@
         <v>136.0</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>25</v>
@@ -6482,7 +6492,7 @@
       </c>
       <c r="E137" s="10"/>
       <c r="F137" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G137" s="10"/>
       <c r="H137" s="8">
@@ -6508,7 +6518,7 @@
         <v>137.0</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C138" s="8" t="s">
         <v>21</v>
@@ -6518,14 +6528,14 @@
       </c>
       <c r="E138" s="10"/>
       <c r="F138" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G138" s="10"/>
       <c r="H138" s="18">
         <v>6.0</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J138" s="10"/>
       <c r="K138" s="17">
@@ -6546,13 +6556,13 @@
         <v>138.0</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C139" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E139" s="10"/>
       <c r="F139" s="14" t="s">
@@ -6563,16 +6573,16 @@
         <v>5.0</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J139" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="K139" s="17">
         <v>0.0</v>
       </c>
       <c r="L139" s="17" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="M139" s="13" t="str">
         <f t="shared" si="3"/>
@@ -6588,13 +6598,13 @@
         <v>139.0</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C140" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E140" s="18" t="s">
         <v>33</v>
@@ -6607,14 +6617,14 @@
         <v>10.0</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J140" s="10"/>
       <c r="K140" s="17">
         <v>1.0</v>
       </c>
       <c r="L140" s="17" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="M140" s="13" t="str">
         <f t="shared" si="3"/>
@@ -6630,33 +6640,33 @@
         <v>140.0</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C141" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E141" s="10"/>
       <c r="F141" s="14" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G141" s="10"/>
       <c r="H141" s="8">
         <v>5.0</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J141" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="K141" s="17">
         <v>0.0</v>
       </c>
       <c r="L141" s="17" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="M141" s="13" t="str">
         <f t="shared" si="3"/>
@@ -6672,33 +6682,33 @@
         <v>141.0</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C142" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E142" s="18" t="s">
         <v>33</v>
       </c>
       <c r="F142" s="16" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="G142" s="10"/>
       <c r="H142" s="8">
         <v>10.0</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="17">
         <v>1.0</v>
       </c>
       <c r="L142" s="17" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="M142" s="13" t="str">
         <f t="shared" si="3"/>
@@ -6714,7 +6724,7 @@
         <v>142.0</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C143" s="8" t="s">
         <v>25</v>
@@ -6723,7 +6733,7 @@
         <v>46</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F143" s="14" t="s">
         <v>64</v>
@@ -6733,14 +6743,14 @@
         <v>11.0</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J143" s="10"/>
       <c r="K143" s="17">
         <v>0.0</v>
       </c>
       <c r="L143" s="17" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="M143" s="13" t="str">
         <f t="shared" si="3"/>
@@ -6756,24 +6766,24 @@
         <v>143.0</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D144" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E144" s="10"/>
       <c r="F144" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G144" s="10"/>
       <c r="H144" s="8">
         <v>11.0</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J144" s="10"/>
       <c r="K144" s="17">
@@ -6796,13 +6806,13 @@
         <v>144.0</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>46</v>
@@ -6811,13 +6821,13 @@
         <v>60</v>
       </c>
       <c r="G145" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H145" s="8">
         <v>11.0</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="17">
@@ -6838,13 +6848,13 @@
         <v>145.0</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E146" s="8" t="s">
         <v>46</v>
@@ -6853,13 +6863,13 @@
         <v>60</v>
       </c>
       <c r="G146" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H146" s="8">
         <v>11.0</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="J146" s="10"/>
       <c r="K146" s="17">
@@ -6880,10 +6890,10 @@
         <v>146.0</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D147" s="8" t="s">
         <v>28</v>
@@ -6901,7 +6911,7 @@
         <v>11.0</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="J147" s="10"/>
       <c r="K147" s="17">
@@ -6922,27 +6932,27 @@
         <v>147.0</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C148" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E148" s="10"/>
       <c r="F148" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G148" s="10"/>
       <c r="H148" s="8">
         <v>4.0</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J148" s="18" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="K148" s="17">
         <v>0.0</v>
@@ -6962,24 +6972,24 @@
         <v>148.0</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C149" s="18" t="s">
         <v>67</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E149" s="10"/>
       <c r="F149" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G149" s="10"/>
       <c r="H149" s="8">
         <v>8.0</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="J149" s="8" t="s">
         <v>23</v>
@@ -7002,17 +7012,17 @@
         <v>149.0</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E150" s="10"/>
       <c r="F150" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G150" s="10"/>
       <c r="H150" s="8">
@@ -7038,17 +7048,17 @@
         <v>150.0</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E151" s="10"/>
       <c r="F151" s="14" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G151" s="10"/>
       <c r="H151" s="8">
@@ -7074,26 +7084,26 @@
         <v>151.0</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E152" s="10"/>
       <c r="F152" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G152" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H152" s="8">
         <v>12.0</v>
       </c>
       <c r="I152" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="J152" s="10"/>
       <c r="K152" s="17">

</xml_diff>